<commit_message>
updated rtm and defect report
</commit_message>
<xml_diff>
--- a/Defect-Report-Lei.xlsx
+++ b/Defect-Report-Lei.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricSuminski\Desktop\matrix-docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frejusgnonsey/Documents/Revature/Lei_FoundationsProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C2538C-564B-4E03-9277-F565A93E662E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25C2879-A805-DD4C-A064-8486E0838B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20740" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Defect ID</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>High</t>
-  </si>
-  <si>
     <t>Medium</t>
   </si>
   <si>
@@ -65,23 +62,20 @@
     <t>Low</t>
   </si>
   <si>
-    <t>Users can log in to the application with only a correct Username</t>
-  </si>
-  <si>
-    <t>Pending</t>
-  </si>
-  <si>
-    <t>The company logo loads in the wrong place</t>
-  </si>
-  <si>
-    <t>Employees are unable to change their personal information on their internal company profile</t>
+    <t>Defects can be successfully reported if steps given are too short, as defect text area does not have minimum characters input</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>Original steps could be replicated on Update case</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,7 +87,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -109,19 +103,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -187,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -202,65 +197,58 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -279,7 +267,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -567,7 +555,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -575,114 +563,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="146.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="2" max="2" width="146.5" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" customWidth="1"/>
+    <col min="6" max="6" width="23.1640625" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
+    <row r="2" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="9">
         <v>901</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="16">
+        <v>809</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="17" t="s">
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10">
+        <v>902</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="26">
-        <v>801</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
-        <v>902</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="20" t="s">
+      <c r="D3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="16">
+        <v>813</v>
+      </c>
+      <c r="F3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="26">
-        <v>805</v>
-      </c>
-      <c r="F3" s="23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
-        <v>903</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="26">
-        <v>805</v>
-      </c>
-      <c r="F4" s="24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="26">
-        <v>806</v>
-      </c>
-      <c r="F5" s="25"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="19"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="17"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="19"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="18"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="6"/>
@@ -690,7 +664,7 @@
       <c r="E6" s="1"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="6"/>
@@ -698,7 +672,7 @@
       <c r="E7" s="1"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="6"/>
@@ -706,7 +680,7 @@
       <c r="E8" s="1"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="6"/>
@@ -715,7 +689,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="1"/>
       <c r="C10" s="6"/>
@@ -723,7 +697,7 @@
       <c r="E10" s="1"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="4"/>
       <c r="C11" s="6"/>
@@ -731,23 +705,13 @@
       <c r="E11" s="1"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="1"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="1"/>
       <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="8"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>